<commit_message>
this is my second commit remaining code are pending for working
</commit_message>
<xml_diff>
--- a/MainController.xlsx
+++ b/MainController.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BSA_MOBILE_FRAMEWORK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92D84FB-531B-47C9-B386-901136F69285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EC35AD-FBF1-4685-8185-27ABCD8C6188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{25C6B8C4-9C4A-44EA-8605-4300C0C3F79D}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="MOBILE_CONFIGURATION" sheetId="3" r:id="rId3"/>
     <sheet name="DB_CONNECTION" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
   <si>
     <t>Si_No</t>
   </si>
@@ -48,9 +48,6 @@
     <t>ExecutionType</t>
   </si>
   <si>
-    <t>ApplicationId</t>
-  </si>
-  <si>
     <t>TestDataSheet</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>FOSs</t>
+  </si>
+  <si>
+    <t>ApplicationName</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,7 +552,7 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -566,7 +566,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -582,10 +582,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E97B1E07-4DA7-41EB-9AFF-2BFFC4045DD0}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -609,13 +609,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -626,15 +626,35 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>20</v>
       </c>
       <c r="F2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
         <v>30</v>
       </c>
     </row>
@@ -680,40 +700,40 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
       <c r="L1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -724,43 +744,43 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H2">
         <v>11</v>
       </c>
       <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="L2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -774,40 +794,40 @@
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H3">
         <v>11</v>
       </c>
       <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="L3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -846,16 +866,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>31</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -869,16 +889,16 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some scroll function
</commit_message>
<xml_diff>
--- a/MainController.xlsx
+++ b/MainController.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BSA_MOBILE_FRAMEWORK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3E927E-37E9-482C-868F-FDE528DE3EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49EDACB-513C-4519-9BFE-361131308C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{25C6B8C4-9C4A-44EA-8605-4300C0C3F79D}"/>
   </bookViews>
@@ -765,7 +765,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add one scroll function and add excel file
</commit_message>
<xml_diff>
--- a/MainController.xlsx
+++ b/MainController.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BSA_MOBILE_FRAMEWORK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49EDACB-513C-4519-9BFE-361131308C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC08D83F-AE27-4A5D-A1A6-B868C031AC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{25C6B8C4-9C4A-44EA-8605-4300C0C3F79D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{25C6B8C4-9C4A-44EA-8605-4300C0C3F79D}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN_CONTROLLER" sheetId="1" r:id="rId1"/>
@@ -208,10 +208,10 @@
     <t>qZHZfSFttvdThCVVX6Ki</t>
   </si>
   <si>
-    <t>FOS3.xlsx</t>
-  </si>
-  <si>
     <t>d4a4d1d2</t>
+  </si>
+  <si>
+    <t>FOS4.xlsx</t>
   </si>
 </sst>
 </file>
@@ -681,7 +681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E97B1E07-4DA7-41EB-9AFF-2BFFC4045DD0}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -746,7 +746,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E3">
         <v>20</v>
@@ -764,7 +764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A659C7-4FC8-47B5-9B4A-1B5BDCE68376}">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -899,7 +899,7 @@
         <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G3" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
total whole code for mobile
</commit_message>
<xml_diff>
--- a/MainController.xlsx
+++ b/MainController.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BSA_MOBILE_FRAMEWORK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA38954-15D0-4FE1-95F6-4453CA798FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C98F62B-5524-40EA-B265-25CC40094DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{25C6B8C4-9C4A-44EA-8605-4300C0C3F79D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{25C6B8C4-9C4A-44EA-8605-4300C0C3F79D}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN_CONTROLLER" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
   <si>
     <t>Si_No</t>
   </si>
@@ -211,7 +211,16 @@
     <t>d4a4d1d2</t>
   </si>
   <si>
-    <t>FOS5.xlsx</t>
+    <t>FOS3.xlsx</t>
+  </si>
+  <si>
+    <t>ApplicationType</t>
+  </si>
+  <si>
+    <t>WEB</t>
+  </si>
+  <si>
+    <t>MOBILE</t>
   </si>
 </sst>
 </file>
@@ -606,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43CBD30-1ED8-4A96-A2D6-7A949A45DBE4}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,10 +627,11 @@
     <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -637,8 +647,11 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -654,8 +667,11 @@
       <c r="E2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -670,6 +686,29 @@
       </c>
       <c r="E3" t="s">
         <v>42</v>
+      </c>
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -681,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E97B1E07-4DA7-41EB-9AFF-2BFFC4045DD0}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
integrate web testing with this framework
</commit_message>
<xml_diff>
--- a/MainController.xlsx
+++ b/MainController.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BSA_MOBILE_FRAMEWORK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C98F62B-5524-40EA-B265-25CC40094DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD779317-D06E-4386-A230-EFF1CCFE9935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{25C6B8C4-9C4A-44EA-8605-4300C0C3F79D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{25C6B8C4-9C4A-44EA-8605-4300C0C3F79D}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN_CONTROLLER" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
   <si>
     <t>Si_No</t>
   </si>
@@ -211,16 +211,13 @@
     <t>d4a4d1d2</t>
   </si>
   <si>
-    <t>FOS3.xlsx</t>
-  </si>
-  <si>
-    <t>ApplicationType</t>
-  </si>
-  <si>
-    <t>WEB</t>
-  </si>
-  <si>
-    <t>MOBILE</t>
+    <t>Ishine</t>
+  </si>
+  <si>
+    <t>Ishine.xlsx</t>
+  </si>
+  <si>
+    <t>FOS8.xlsx</t>
   </si>
 </sst>
 </file>
@@ -266,12 +263,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -287,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -300,6 +303,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -615,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43CBD30-1ED8-4A96-A2D6-7A949A45DBE4}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -628,10 +632,9 @@
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -647,11 +650,8 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -667,15 +667,12 @@
       <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C3" t="s">
@@ -687,28 +684,39 @@
       <c r="E3" t="s">
         <v>42</v>
       </c>
-      <c r="F3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -718,10 +726,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E97B1E07-4DA7-41EB-9AFF-2BFFC4045DD0}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -785,12 +793,32 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
         <v>20</v>
       </c>
     </row>
@@ -803,7 +831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A659C7-4FC8-47B5-9B4A-1B5BDCE68376}">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -980,7 +1008,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
complete user2 qc excel sheet
</commit_message>
<xml_diff>
--- a/MainController.xlsx
+++ b/MainController.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BSA_MOBILE_FRAMEWORK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95AD2EC9-44FC-44E8-82C5-141A9180D6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529FF898-906A-43B8-B7F6-77B6D6BFABCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{25C6B8C4-9C4A-44EA-8605-4300C0C3F79D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{25C6B8C4-9C4A-44EA-8605-4300C0C3F79D}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN_CONTROLLER" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="73">
   <si>
     <t>Si_No</t>
   </si>
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43CBD30-1ED8-4A96-A2D6-7A949A45DBE4}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -769,7 +769,7 @@
         <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
@@ -779,6 +779,23 @@
       </c>
       <c r="E6" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -794,10 +811,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E97B1E07-4DA7-41EB-9AFF-2BFFC4045DD0}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -937,36 +954,16 @@
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>62</v>
+      <c r="C7" t="s">
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
       <c r="F7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8">
-        <v>10</v>
-      </c>
-      <c r="F8">
         <v>20</v>
       </c>
     </row>

</xml_diff>